<commit_message>
Front-End Tests + A few Back Impls
</commit_message>
<xml_diff>
--- a/Tarefas.xlsx
+++ b/Tarefas.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tarefas" sheetId="1" r:id="Rc33fd8bd3f72439b"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tarefas" sheetId="1" r:id="Raee9f6beb9f0428d"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -45,94 +45,97 @@
         <x:v>Total do Período</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>sáb 01/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>dom 02/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>seg 03/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>ter 04/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>qua 05/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>qui 06/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>sex 07/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>sáb 08/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>dom 09/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>seg 10/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>ter 11/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>qua 12/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>qui 13/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>sex 14/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>sáb 15/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>dom 16/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>seg 17/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>ter 18/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>qua 19/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>qui 20/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>sex 21/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>sáb 22/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>dom 23/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>seg 24/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>ter 25/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>qua 26/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>qui 27/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>sex 28/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>sáb 29/04</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>dom 30/04</x:v>
+        <x:v>seg 01/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>ter 02/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>qua 03/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>qui 04/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>sex 05/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>sáb 06/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>dom 07/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>seg 08/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>ter 09/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>qua 10/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>qui 11/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>sex 12/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>sáb 13/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>dom 14/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>seg 15/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>ter 16/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>qua 17/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>qui 18/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>sex 19/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>sáb 20/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>dom 21/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>seg 22/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>ter 23/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>qua 24/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>qui 25/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>sex 26/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>sáb 27/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>dom 28/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>seg 29/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>ter 30/05</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>qua 31/05</x:v>
       </x:c>
     </x:row>
     <x:row>
@@ -259,6 +262,9 @@
       <x:c t="str">
         <x:v/>
       </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
@@ -384,6 +390,9 @@
       <x:c t="str">
         <x:v/>
       </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
@@ -509,6 +518,9 @@
       <x:c t="str">
         <x:v/>
       </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
@@ -634,6 +646,9 @@
       <x:c t="str">
         <x:v/>
       </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
@@ -759,6 +774,9 @@
       <x:c t="str">
         <x:v/>
       </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
@@ -884,6 +902,9 @@
       <x:c t="str">
         <x:v>0h</x:v>
       </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
@@ -1009,6 +1030,9 @@
       <x:c t="str">
         <x:v>0h</x:v>
       </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
@@ -1033,7 +1057,10 @@
         <x:v>28/07/2022</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>90,4h</x:v>
+        <x:v>91,4h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
       </x:c>
       <x:c t="str">
         <x:v/>
@@ -1158,7 +1185,10 @@
         <x:v>28/07/2022</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>90,4h</x:v>
+        <x:v>91,4h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
       </x:c>
       <x:c t="str">
         <x:v/>
@@ -1349,40 +1379,43 @@
         <x:v>0h</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
       </x:c>
     </x:row>
     <x:row>
@@ -1417,67 +1450,70 @@
         <x:v>0026_001</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>1h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>1h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
       </x:c>
       <x:c t="str">
         <x:v/>
@@ -1521,7 +1557,7 @@
         <x:v>Reunião Tribo ou Retro tribo/squads</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>Aguardando Aprovação</x:v>
+        <x:v>Atualizada pelo Gerente</x:v>
       </x:c>
       <x:c t="str">
         <x:v>0h</x:v>
@@ -1533,7 +1569,7 @@
         <x:v>01/08/2022</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>33h</x:v>
+        <x:v>34h</x:v>
       </x:c>
       <x:c t="str">
         <x:v>Tribo E&amp;S - Estudo/projetos internos &gt; Devero</x:v>
@@ -1542,58 +1578,61 @@
         <x:v>0026_001</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>3h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>1h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>1h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>1h</x:v>
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
       </x:c>
       <x:c t="str">
         <x:v/>
@@ -1646,7 +1685,7 @@
         <x:v>KXs</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>Aguardando Aprovação</x:v>
+        <x:v>Atualizada pelo Gerente</x:v>
       </x:c>
       <x:c t="str">
         <x:v>18h</x:v>
@@ -1667,58 +1706,61 @@
         <x:v>0026_001</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
       </x:c>
       <x:c t="str">
         <x:v>0h</x:v>
@@ -1792,25 +1834,28 @@
         <x:v>0026_001</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
       </x:c>
       <x:c t="str">
         <x:v>0h</x:v>
@@ -1896,7 +1941,7 @@
         <x:v>Atividades RH da Tribo</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>Aguardando Aprovação</x:v>
+        <x:v>Atualizada pelo Gerente</x:v>
       </x:c>
       <x:c t="str">
         <x:v>21h</x:v>
@@ -1917,61 +1962,64 @@
         <x:v>0026_001</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
       </x:c>
       <x:c t="str">
         <x:v>0h</x:v>
@@ -2024,7 +2072,7 @@
         <x:v/>
       </x:c>
       <x:c t="str">
-        <x:v>21,2h</x:v>
+        <x:v>9,7h</x:v>
       </x:c>
       <x:c t="str">
         <x:v/>
@@ -2033,7 +2081,10 @@
         <x:v>03/01/2022</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>1.761,4h</x:v>
+        <x:v>1.808,5h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
       </x:c>
       <x:c t="str">
         <x:v/>
@@ -2149,7 +2200,7 @@
         <x:v/>
       </x:c>
       <x:c t="str">
-        <x:v>21,2h</x:v>
+        <x:v>9,7h</x:v>
       </x:c>
       <x:c t="str">
         <x:v/>
@@ -2158,7 +2209,10 @@
         <x:v>03/01/2022</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>1.761,4h</x:v>
+        <x:v>1.808,5h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
       </x:c>
       <x:c t="str">
         <x:v/>
@@ -2271,7 +2325,7 @@
         <x:v> DSM</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>Aguardando Aprovação</x:v>
+        <x:v>Atualizada pelo Gerente</x:v>
       </x:c>
       <x:c t="str">
         <x:v>0h</x:v>
@@ -2283,7 +2337,7 @@
         <x:v>03/01/2022</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>125,5h</x:v>
+        <x:v>128,5h</x:v>
       </x:c>
       <x:c t="str">
         <x:v>DeVero &gt; Atividades Gerais</x:v>
@@ -2292,67 +2346,70 @@
         <x:v>8121_001</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>7h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
         <x:v>1h</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>1h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
       </x:c>
       <x:c t="str">
         <x:v/>
@@ -2396,7 +2453,7 @@
         <x:v> Melhorias ArcelorMittal</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>Aguardando Aprovação</x:v>
+        <x:v>Atualizada pelo Gerente</x:v>
       </x:c>
       <x:c t="str">
         <x:v>0h</x:v>
@@ -2408,7 +2465,7 @@
         <x:v>03/01/2022</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>793,7h</x:v>
+        <x:v>814,3h</x:v>
       </x:c>
       <x:c t="str">
         <x:v>DeVero &gt; Atividades Gerais</x:v>
@@ -2417,61 +2474,64 @@
         <x:v>8121_001</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>9,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>1h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>4,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>4h</x:v>
+        <x:v>3,6h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>3,6h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
       </x:c>
       <x:c t="str">
         <x:v/>
@@ -2521,7 +2581,7 @@
         <x:v> Avaliação de PR</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>Aguardando Aprovação</x:v>
+        <x:v>Atualizada pelo Gerente</x:v>
       </x:c>
       <x:c t="str">
         <x:v>0h</x:v>
@@ -2533,7 +2593,7 @@
         <x:v>14/01/2022</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>97,1h</x:v>
+        <x:v>99,1h</x:v>
       </x:c>
       <x:c t="str">
         <x:v>DeVero &gt; Atividades Gerais</x:v>
@@ -2542,64 +2602,67 @@
         <x:v>8121_001</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>5,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
         <x:v>0,5h</x:v>
       </x:c>
       <x:c t="str">
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
         <x:v>0,5h</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0,5h</x:v>
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
       </x:c>
       <x:c t="str">
         <x:v/>
@@ -2759,6 +2822,9 @@
       <x:c t="str">
         <x:v/>
       </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
@@ -2771,7 +2837,7 @@
         <x:v> Melhorias Viridis</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>Aguardando Aprovação</x:v>
+        <x:v>Atualizada pelo Gerente</x:v>
       </x:c>
       <x:c t="str">
         <x:v>0h</x:v>
@@ -2783,7 +2849,7 @@
         <x:v>04/02/2022</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>458,8h</x:v>
+        <x:v>461,8h</x:v>
       </x:c>
       <x:c t="str">
         <x:v>DeVero &gt; Atividades Gerais</x:v>
@@ -2792,67 +2858,70 @@
         <x:v>8121_001</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>54,3h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>6,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>7,1h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>6,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>6,6h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
         <x:v>3h</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>3,7h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>4,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>6,9h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>1h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>2,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>1h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
+        <x:v>0h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>3h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
       </x:c>
       <x:c t="str">
         <x:v/>
@@ -2899,22 +2968,25 @@
         <x:v>Atualizada pelo Gerente</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>21,2h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>47%</x:v>
+        <x:v>9,7h</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>76%</x:v>
       </x:c>
       <x:c t="str">
         <x:v>03/03/2022</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>18,8h</x:v>
+        <x:v>30,3h</x:v>
       </x:c>
       <x:c t="str">
         <x:v>DeVero &gt; Atividades Gerais</x:v>
       </x:c>
       <x:c t="str">
         <x:v>8121_001</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>0h</x:v>
       </x:c>
       <x:c t="str">
         <x:v>0h</x:v>
@@ -3021,7 +3093,7 @@
         <x:v> Correções de erros no Viridis</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>Aguardando Aprovação</x:v>
+        <x:v>Atualizada pelo Gerente</x:v>
       </x:c>
       <x:c t="str">
         <x:v>0h</x:v>
@@ -3033,7 +3105,7 @@
         <x:v>03/03/2022</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>250,5h</x:v>
+        <x:v>257,5h</x:v>
       </x:c>
       <x:c t="str">
         <x:v>DeVero &gt; Atividades Gerais</x:v>
@@ -3042,67 +3114,70 @@
         <x:v>8121_001</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>23h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>3h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>3h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>3h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>0h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>6,5h</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>7,5h</x:v>
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
+      </x:c>
+      <x:c t="str">
+        <x:v/>
       </x:c>
       <x:c t="str">
         <x:v/>

</xml_diff>